<commit_message>
added the logic for parsing basic datatypes will need some error handling eventually
</commit_message>
<xml_diff>
--- a/Input Files/testtable.xlsx
+++ b/Input Files/testtable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billy\Desktop\Projects\Database-Migrate\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605AECB0-D400-4F6D-8863-B5F18767FBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231AE5CD-67D4-43D7-80AF-3B3CC0AF53D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -40,12 +40,30 @@
   </si>
   <si>
     <t>samir</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>decimal_int</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,8 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,15 +377,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,8 +400,23 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -386,8 +426,23 @@
       <c r="C2">
         <v>21</v>
       </c>
+      <c r="D2" s="1">
+        <v>45500</v>
+      </c>
+      <c r="E2">
+        <v>1.3</v>
+      </c>
+      <c r="F2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45500.083333333336</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45500</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -396,6 +451,21 @@
       </c>
       <c r="C3">
         <v>20</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45500</v>
+      </c>
+      <c r="E3">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>1.2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45500</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>